<commit_message>
DB - Data Access with ADO.NET -HW -U
</commit_message>
<xml_diff>
--- a/Databases/07. Data Access with ADO.NET/07. Write to Excel/db.xlsx
+++ b/Databases/07. Data Access with ADO.NET/07. Write to Excel/db.xlsx
@@ -408,10 +408,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <dimension ref="A1:B16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
@@ -420,7 +420,7 @@
     <col min="1" max="1" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row spans="1:2" x14ac:dyDescent="0.25" outlineLevel="0" r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -428,7 +428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row spans="1:2" x14ac:dyDescent="0.25" outlineLevel="0" r="2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -436,7 +436,7 @@
         <v>25</v>
       </c>
     </row>
-    <row spans="1:2" x14ac:dyDescent="0.25" outlineLevel="0" r="3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -444,7 +444,7 @@
         <v>22</v>
       </c>
     </row>
-    <row spans="1:2" x14ac:dyDescent="0.25" outlineLevel="0" r="4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -452,7 +452,7 @@
         <v>24</v>
       </c>
     </row>
-    <row spans="1:2" x14ac:dyDescent="0.25" outlineLevel="0" r="5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -460,112 +460,12 @@
         <v>20</v>
       </c>
     </row>
-    <row spans="1:2" x14ac:dyDescent="0.25" outlineLevel="0" r="6">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="3">
         <v>33</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="7">
-      <c r="A7" s="3" t="inlineStr">
-        <is>
-          <t>Peter Ivanov</t>
-        </is>
-      </c>
-      <c r="B7" s="3">
-        <v>25</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="8">
-      <c r="A8" s="3" t="inlineStr">
-        <is>
-          <t>Peter Ivanov</t>
-        </is>
-      </c>
-      <c r="B8" s="3">
-        <v>25</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="9">
-      <c r="A9" s="3" t="inlineStr">
-        <is>
-          <t>Peter Ivanov</t>
-        </is>
-      </c>
-      <c r="B9" s="3">
-        <v>25</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="10">
-      <c r="A10" s="3" t="inlineStr">
-        <is>
-          <t>Peter Ivanov</t>
-        </is>
-      </c>
-      <c r="B10" s="3">
-        <v>25</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="11">
-      <c r="A11" s="3" t="inlineStr">
-        <is>
-          <t>Peter Ivanov</t>
-        </is>
-      </c>
-      <c r="B11" s="3">
-        <v>25</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="12">
-      <c r="A12" s="3" t="inlineStr">
-        <is>
-          <t>Peter Ivanov</t>
-        </is>
-      </c>
-      <c r="B12" s="3">
-        <v>25</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="13">
-      <c r="A13" s="3" t="inlineStr">
-        <is>
-          <t>Peter Ivanov</t>
-        </is>
-      </c>
-      <c r="B13" s="3">
-        <v>25</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="14">
-      <c r="A14" s="3" t="inlineStr">
-        <is>
-          <t>Peter Ivanov</t>
-        </is>
-      </c>
-      <c r="B14" s="3">
-        <v>25</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="15">
-      <c r="A15" s="3" t="inlineStr">
-        <is>
-          <t>Peter Ivanov</t>
-        </is>
-      </c>
-      <c r="B15" s="3">
-        <v>25</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="16">
-      <c r="A16" s="3" t="inlineStr">
-        <is>
-          <t>Peter Ivanov</t>
-        </is>
-      </c>
-      <c r="B16" s="3">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>